<commit_message>
handling of empty param value added.
</commit_message>
<xml_diff>
--- a/GeneralApiTest/resources/selfTest.xlsx
+++ b/GeneralApiTest/resources/selfTest.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="orderId" localSheetId="0">Sheet1!$D$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>U1</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>{"code":200,"data":{"code":"IN","name":"India","states":[{"code":"AP","cities":["Yanam","Vizianagaram","Visakhapatnam","Vinukonda","Vijayawada","Tirumala - Tirupati","Tirumala","Thenali","Tanuku","Tadepallegudem","Srikakulam","Singarayakonda","Ramavaram","Ramapuram","Rajahmundry","Puttur","Proddatur","Pithapuram","Pileru","Piduguralla","Peddapuram","Pakala","Ongole","Nuzvid","Nellore","Narasaraopet","Nandyal","Nandigama","Nagari","Muddanuru","Medarametla","Markapur","Mangalagiri","Mandapeta","Mahal","Madanapalle","Machilipatnam","Kurnool","Kuppam","Kovvur","Kavali","Kanigiri","Kakinada","Guntur","Gudivada","Gorantla","Gannavaram","Gampalagudem","Eluru","Dhone","Darsi","Cumbum","Kadapa","Chittoor","Chirala","Bobbili","Bhimavaram","Bapatla","Avanigadda","Andra","Anantapur","Amalapuram","Akividu"],"name":"Andhra Pradesh"},{"code":"AR","cities":["Itanagar","Hong"],"name":"Arunachal Pradesh"},{"code":"AS","cities":["Ulubari","Tinsukia","Tezpur","Silchar","Sibsagar","Powai","North Lakhimpur","Nazira","Namrup","Nalbari","Lala","Kokrajhar","Karimganj","Jorhat","Goshaingaon","Golaghat","Guwahati","Dibrugarh","Dhubri","Bhandari","Barpeta","Arunachal"],"name":"Assam"},{"code":"BR","cities":["Samastipur","Sakri","Raxaul","Pusa","Patna","Muzaffarpur","Munger","Motihari","Kamat","Jha Jha","Jaynagar","Gaya","Dhaka","Darbhanga","Chandan","Bihar Sharif","Bhawanipur","Bhagalpur","Begusarai","Banka","Purnea"],"name":"Bihar"},{"code":"CH","cities":["Chandigarh"],"name":"Chandigarh"},{"code":"DN","cities":["Silvassa","Amal"],"name":"Dadra and Nagar Haveli"},{"code":"DD","cities":["Daman"],"name":"Daman and Diu"},{"code":"GA","cities":["Verna","Vasco","Vainguinim","Solim","Sanquelim","Saligao","Quepem","Ponda","Parra","Panjim","Navelim","Marmagao","Madgaon","Goa","Dona Paula","Dicholi","Curchorem","Cuncolim","Calangute","Chicalim","Caranzalem","Candolim","Betim","Betalbatim","Bambolim","Assagao","Arpora","Aldona"],"name":"Goa"},{"code":"GJ","cities":["Vadodra","Visnagar","Vijapur","Valsad","Vadodara","Thasra","Surendranagar","Somnath","Sanand","Sami","Sachin","Rawal","Rander","Rajkot","Porbandar","Petlad","Patan","Navsari","Nagwa","Nadiad","Mundra","Morvi","Modasa","Mithapur","Matar","Mandvi","Malpur","Mahesana","Kosamba","Khergam","Kheda","Khambhat","Keshod","Karamsad","Kalol","Junagadh","Jamnagar","Jalalpur","Himatnagar","Godhra","Ghana","Gandhinagar","Gandhidham","Dwarka","Dhrol","Dhansura","Dewan","Dahod","Chhota Udepur","Bilimora","Bhuj","Bhavnagar","Bharuch","Bhadath","Basu","Bardoli","Antapur","Ankleshwar","Anand","Amroli","Amreli","Ahmedabad","Vapi"],"name":"Gujarat"},{"code":"HR","cities":["Yamunanagar","Tohana","Sonipat","Sirsa","Shahabad","Saha","Rohtak","Rewari","Pehowa","Panipat","Palwal","Odhan","Nilokheri","Narnaul","Ladwa","Kaul","Karnal","Kaithal","Jind","Jhajjar","Indraprast","Hisar","Hansi","Gurgaon","Gohana","Ganga","Fatehabad","Faridabad","Chhachhrauli","Bhiwani","Ballabgarh","Bahadurgarh","Aurangabad","Ambala","Sodhi","Haryana","Budha","Kalra","Kotian"],"name":"Haryana"},{"code":"KA","cities":["Yadgir","Udupi","Tumk?r","Tiptur","Someshwar","Siruguppa","Sirsi","Shimoga","Sangam","Sandur","Sagar","Ramanagaram","Raichur","Puttur","Nandi","Mysore","Mundgod","Manipala","Mangalore","Mandya","Madikeri","Kushalnagar","Koppal","Kollegal","Kolar","Karwar","Hubli","Hospet","Honavar","Hiriyur","Hira","Haveri","Hassan","Hadadi","Gulbarga","Shanti Grama","Gadag","Dharwad","Davangere","Chitradurga","Chintamani","Chikodi","Chikmagal?r","Channapatna","Bijapur","Bidar","Bhatkal","Bhadravati","Bellary","Bellare","Belgaum","Bangalore","Bagalkot"],"name":"Karnataka"},{"code":"JK","cities":["Srinagar","Ring","Pahalgam","Katra","Kathua","Kargil","Jammu","Bawan","Anantnag","Markal","Nila","Arch","Gold","Raju","Kundan","Suman","Bala","Patel","Ranjan"],"name":"Kashmir"},{"code":"KL","cities":["Vazhakulam","Vaikam","Thiruvananthapuram","Thrissur","Tiruvalla","Tirur","Thalassery","Sultans Battery","Shoranur","Kollam","Punalur","Ponnani","Payyanur","Pattambi","Pathanamthitta","Paravur","Parappanangadi","Palakkad","Palayam","Ottappalam","Nilambur","Mavelikara","Mattanur","Manjeri","Malappuram","Kozhikode","Kottayam","Kottarakara","Kottakkal","Koni","Kodungallur","Kayamkulam","Kasaragod","Kanhangad","Kalpetta","Kaladi","Irinjalakuda","Idukki","Guruvayur","Ernakulam","Edavanna","Kochi","Chittur","Chengannur","Changanacheri","Kannur","Attingal","Aranmula","Angadipuram","Anchal","Aluva","Alappuzha","Alanallur"],"name":"Kerala"},{"code":"LD","cities":["Kavaratti"],"name":"Laccadives"},{"code":"MP","cities":["Vidisha","Ujjain","Tala","Soni","Sidhi","Shahdol","Sendhwa","Sehore","Satna","Sarangi","Sagar","Rewa","Ratlam","Rama","Raipur","Pachmarhi","Morena","Mhow","Mandsaur","Mandla","Khargone","Khajuraho Group of Monuments","Katni","Kataria","Kailaras","Jabalpur","Indore","Hoshangabad","Gwalior","Guna","Dindori","Dhar","Dewas","Damoh","Chhindwara","Chand","Bhopal","Betul","Berasia","Baroda","Balaghat","Bagh","Anantpur","Ambah","Amarkantak","Ganpat","Nadia","Chakra","Bhartiya","Gandhigram","Kamalpura","Rajapur","Nagara","Chopra","Bhagwan"],"name":"Madhya Pradesh"},{"code":"MH","cities":["Yeola","Yavatmal","Wardha","Wai","Virar","Vashi","Vasai","Vadner","Umred","Ulhasnagar","Tuljapur","Trimbak","Thane","Talegaon Dabhade","Sopara","Sion","Sinnar","Shrigonda","Solapur","Shirgaon","Shahapur","Satara","Sangola","Sangli","Sangamner","Sakri","Ratnagiri","Puras","Pune","Pimpri","Parel","Parbhani","Panvel","Pandharpur","Panchgani","Palus","Palghar","Osmanabad","Neri","Neral","Nashik","Narayangaon","Nandurbar","Nanded","Nagpur","Nadgaon","Miraj","Manor","Mangaon","Mahim","Mahad","Latur","Kolhapur","Khopoli","Khalapur","Karjat","Karanja","Karad","Kankauli","Kalyan","Kalamboli","Kalam","Kagal","Jalna","Jalgaon Jamod","Igatpuri","Ichalkaranji","Hingoli","Hinganghat","Goregaon","Ghatkopar","Gargoti","Ellora Caves","Dhule","Dharavi","Devgarh","Deolali","Dahanu","Colaba","Chopda","Chiplun","Chinchvad","Charan","Chandrapur","Chalisgaon","Chakan","Mumbai","Boisar","Bhusawal","Bhiwandi","Bhandup","Belapur","Baramati","Badlapur","Aurangabad","Aundh","Arvi","Andheri","Amravati","Ambad","Ambarnath","Alibag","Akola","Ahmednagar","Abdul","Bandra"],"name":"Maharashtra"},{"code":"MN","cities":["Imphal","Churachandpur"],"name":"Manipur"},{"code":"ML","cities":["Tura","Shillong","Pala","Nongstoin","Nongpoh"],"name":"Meghalaya"},{"code":"MZ","cities":["Aizawl"],"name":"Mizoram"},{"code":"NL","cities":["Kohima","Dimapur","Chen"],"name":"Nagaland"},{"code":"DL","cities":["Shahdara","New Delhi","Narela","Kalkaji Devi","Delhi","Connaught Place","Bawana","Alipur"],"name":"National Capital Territory of Delhi"},{"code":"OR","cities":["Udaigiri","Talcher","Sundargarh","Sambalpur","Rayagada","Raurkela","Puri","Nayagarh","Koraput","Khurda","Kalinga","Jharsuguda","Jaypur","Jatani","Jajpur","Dhenkanal","Cuttack","Brahmapur","Bhubaneswar","Barpali","Bargarh","Balasore","Balangir","Angul"],"name":"Odisha"},{"code":"RJ","cities":["Udaipur","Tonk","Suratgarh","Surana","Sultan","Sojat","Sirohi","Sikar","Shiv","Roshan","Pushkar","Pilani","Pali","Nathdwara","Naraina","Nagaur","Nagar","Manna","Mandal","Mahajan","Lamba Harisingh","Kota","Kolayat","Kishangarh","Khinwara","Jodhpur","Jhunjhunun","Jhalawar","Jaisalmer","Jaipur","Gangrar","Gangapur","Ganganagar","Dipas","Chhabra","Bundi","Binavas","Bikaner","Bhilwara","Bharatpur","Beawar","Barmer","Banswara","Bali","Balana","Amet","Amer","Alwar","Ajmer","Mount Abu","Pitampura","Nanda","Chetan","Thali","Mahatma","Kanakpura","Rana","Charu","Khan","Kalan"],"name":"Rajasthan"},{"code":"SK","cities":["Sirwani","Singtam","Manu","Gangtok"],"name":"Sikkim"},{"code":"CT","cities":["Sukma","Raipur","Raigarh","Mohala","Lanka","Kumhari","Korba","Koni","Janjgir","Jagdalpur","Durg","Dhamtari","Champa","Bilaspur","Bhilai","Bhatapara","Bemetara","Ambikapur"],"name":"State of Chhattisgarh"},{"code":"HP","cities":["Solan","Shimla","Paonta Sahib","Palampur","Nurpur","Nalagarh","Mashobra","Mani","Mandi","Manali","Kumar","Kangra","Kalka","Hari","Hamirpur","Dharamsala","Dharmpur","Chamba","Bilaspur","Bhawan","Nehra"],"name":"State of Himachal Pradesh"},{"code":"JH","cities":["Ranchi","Ramgarh","Mahulia","Jamshedpur","Hazaribagh","Dumka","Dhanbad","Bokaro"],"name":"State of Jharkhand"},{"code":"PB","cities":["Tarn Taran","Talwandi Sabo","Sunam","Sirhind","Shahkot","Sangrur","Rupnagar","Rajpura","Phagwara","Patiala","Pathankot","Nabha","Morinda","Muktsar","Mukerian","Moga","Mansa","Maharaj","Machhiwara","Ludhiana","Kurali","Kot Isa Khan","Kharar","Khanna","Kapurthala Town","Jalandhar","Jalalabad","Jagraon","Hoshiarpur","Gurdaspur","Garhshankar","Firozpur","Faridkot","Dinanagar","Dhuri","Dhariwal","Dasua","Bhatinda","Batala","Barnala","Banga","Amritsar","Mohali"],"name":"State of Punjab"},{"code":"TN","cities":["Yercaud","Wellington","Villupuram","Vellore","Vaniyambadi","Vandavasi","Vandalur","Vadamadurai","Ooty","Turaiyur","Cheyyar","Tiruvannamalai","Tiruvallur","Thiruthani","Tiruppur","Tirunelveli","Tiruchi","Tiruchchendur","Tindivanam","Thiruvarur","Thanjavur","Thenkasi","Tambaram","Srivilliputhur","Srirangam","Sriperumbudur","Sivakasi","Sivaganga","Sirkazhi","Sattur","Salem","Ranippettai","Ramanathapuram","Rajapalaiyam","Puliyur","Pudukkottai","Ponneri","Pollachi","Perundurai","Peranampattu","Perambalur","Pattukkottai","Panruti","Palani","Palladam","Omalur","Neyveli","Namakkal","Nagercoil","Nagapattinam","Mylapore","Mettur","Mannargudi","Mahabalipuram","Madurantakam","Madurai","Chennai","Lalgudi","Kuzhithurai","Koothanallur","Kumbakonam","Krishnagiri","Kovilpatti","Kodaikanal","Karur","Karamadai","Karaikudi","Kanniyakumari","Kaniyambadi","Kangayam","Kanchipuram","Kalpakkam","Hosur","Guindy","Gobichettipalayam","Fort","Erode","Eral","Dindigul","Dharmapuri","Dharapuram","Devipattinam","Cuddalore","Coonoor","Coimbatore","Sholavandan","Chidambaram","Bodinayakkanur","Attur","Ariyalur","Arani","Arakkonam","Annamalainagar","Ambur","Alangulam","Thirumangalam","Choolai","Ekkattuthangal","Siruseri","Thoothukudi"],"name":"Tamil Nadu"},{"code":"TS","cities":["Warangal","Vikarabad","Uppal","Suriapet","Secunderabad","Patancheru","Paloncha","Nizamabad","Nalgonda","Medchal","Medak","Mancherial","Kottagudem","Khammam","Karimnagar","Hyderabad","Gudur","Bodhan","Bhongir","Balanagar","Adilabad","Shadnagar","Patelguda","Pochampalli","Narsapur"],"name":"Telangana"},{"code":"TR","cities":["Kamalpur","Agartala"],"name":"Tripura"},{"code":"AN","cities":["Sawi","Port Blair","Maru"],"name":"Union Territory of Andaman and Nicobar Islands"},{"code":"PY","cities":["Puducherry","Karaikal"],"name":"Union Territory of Puducherry"},{"code":"UP","cities":["Varanasi","Unnao","Tikamgarh","Tanda","Sultanpur","Sitapur","Shamsabad","Shahjahanpur","Sahibabad","Saharanpur","Rampur","Pilkhuwa","Phaphamau","Padrauna","Orai","Muzaffarnagar","Moradabad","Mohan","Mirzapur","Mirza Murad","Meerut","Mawana","Mathura","Madhoganj","Lucknow","Lakhimpur","Kunwar","Khurja","Kheri","Khatauli","Khandar","Kasia","Kasganj","Karari","Kanpur","Kaimganj","Jhansi","Jaunpur","Jalesar","Iglas","Hapur","Hamirpur","Gorakhpur","Gonda","Ghaziabad","Firozabad","Fatehpur","Fatehgarh","Faizabad","Etawah","Deoria","Dasna","Dadri","Chandausi","Chandauli","Bulandshahr","Budaun","Bhadohi","Bela","Basti","Bareilly","Banda","Bagpat","Azamgarh","Anandnagar","Allahabad","Aligarh","Agra","Balu","Sikka","Chitra","Arora","Ajabpur","Bank","Bichpuri","Mehra","Teri","Mathan","Potti","Noida"],"name":"Uttar Pradesh"},{"code":"UL","cities":["Uttarkashi","Roorkee","Rishikesh","Ramnagar","Pithoragarh","Pauri","Pantnagar","Nagal","Mussoorie","Lohaghat","Kashipur","Jaspur","Haridwar","Haldwani","Dwarahat","Dogadda","Dhanaulti","Dang","Vikasnagar","Almora","Adwani","Mill","Naini","Dangi","Jamal","Sidhpur","Dehradun"],"name":"Uttarakhand"},{"code":"WB","cities":["Siuri","Shyamnagar","Serampore","Siliguri","Salt Lake City","Rupnarayanpur","Raniganj","Ranaghat","Puruliya","Panchal","Nabadwip","Murshidabad","Medinipur","Mayapur","Maldah","Liluah","Kulti","Konnagar","Koch Bihar","Kharagpur","Katoya","Karsiyang","Kandi","Kalyani","Kakdwip","Kanchrapara","Jhargram","Jayanti","Jalpaiguri","Jadabpur","Hugli","Howrah","Habra","Ghatal","Farakka","Durgapur","Dam Dam","Darjeeling","Chandannagar","Canning","Kolkata","Budbud","Bolpur","Bishnupur","Binnaguri","Belgharia","Behala","Basirhat","Barddhaman","Barakpur","Bankura","Bangaon","Balurghat","Bali","Baidyabati","Baharampur","Asansol","Alipur","Haldia","Haripur","Rudrapur","Saranga","Rajpur","Gujrat","Multi","Manipur"],"name":"West Bengal"}]},"status":"success"}</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>{"code":"200","data":{"total":3,"start":0,"count":3,"data":[{"supc":"SDL002940000","sellerCode":"8f7f72","name":"NM_Mobile1","pogId":621051679590,"sellerName":null,"price":0,"inventory":0,"offerPrice":0,"live":false,"imgs":null,"pageUrl":"product/nmmobile1/621051679590","category":null,"nodePath":null,"sdplus":false,"shippingDays":0,"productDesc":null,"rating":0.0,"noOfRating":0,"discount":0,"soldOut":true,"brand":"Apple","adCreated":false,"attributes":[]},{"supc":"SDL006331689","sellerCode":"8f7f72","name":"NM_Mobile1","pogId":621051679590,"sellerName":"Spice Retail Ltd.","price":2000,"inventory":200,"offerPrice":2000,"live":true,"imgs":["http://release.sdlcdn.com/http://sdstg.s3.amazonaws.com/imgs/a/a/q/NM-Mobile1-SDL006331689-1-63800.jpg"],"pageUrl":"product/nmmobile1/621051679590","category":null,"nodePath":null,"sdplus":false,"shippingDays":0,"productDesc":null,"rating":0.0,"noOfRating":0,"discount":0,"soldOut":false,"brand":"Apple","adCreated":false,"attributes":[{"name":"Color","value":"Red"}]},{"supc":"SDL000363340","sellerCode":"8f7f72","name":"NM_Mobile1","pogId":621051679590,"sellerName":"Spice Retail Ltd.","price":2000,"inventory":200,"offerPrice":2000,"live":false,"imgs":null,"pageUrl":"product/nmmobile1/621051679590","category":null,"nodePath":null,"sdplus":false,"shippingDays":0,"productDesc":null,"rating":0.0,"noOfRating":0,"discount":0,"soldOut":false,"brand":"Apple","adCreated":false,"attributes":[]}]},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -109,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +138,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -162,6 +178,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -466,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +653,17 @@
       </c>
       <c r="C14" s="4" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>